<commit_message>
fixed discharge issue in DASH survey123 form
</commit_message>
<xml_diff>
--- a/inst/survey_templates/DASH_MasterV9.xlsx
+++ b/inst/survey_templates/DASH_MasterV9.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{609E33A3-51D9-4892-83CA-F58D29B1124A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2DC729CD-8D41-4059-B336-6AAC7A0E4C38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="542" xr2:uid="{C50DDC91-227D-4C28-807B-6890084E472E}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="542" xr2:uid="{C50DDC91-227D-4C28-807B-6890084E472E}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="10" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2124" uniqueCount="1714">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2124" uniqueCount="1713">
   <si>
     <t>Question type</t>
   </si>
@@ -4840,12 +4840,6 @@
     <t>Width should be btw 0 and 3</t>
   </si>
   <si>
-    <t>Width should be btw 0 and 25</t>
-  </si>
-  <si>
-    <t>.&gt;0 and .&lt;=25</t>
-  </si>
-  <si>
     <t>.&gt;0 and .&lt;=3</t>
   </si>
   <si>
@@ -5110,18 +5104,12 @@
     <t>selected(${CU_Type}, 'Riffle') or selected(${CU_Type}, 'Rapid+')</t>
   </si>
   <si>
-    <t>Width should be btw 0 and 5</t>
-  </si>
-  <si>
     <t>Depth should be btw 0 and 3</t>
   </si>
   <si>
     <t>Velocity should be btw -1 and 10</t>
   </si>
   <si>
-    <t>.&gt;0 and .&lt;=5</t>
-  </si>
-  <si>
     <t>.&gt;-1 and .&lt;=10</t>
   </si>
   <si>
@@ -5249,6 +5237,15 @@
   </si>
   <si>
     <t>string-length(${TapeDistance}) &gt; 0</t>
+  </si>
+  <si>
+    <t>Tape distance should be btw 0 and 50</t>
+  </si>
+  <si>
+    <t>.&gt;=0 and .&lt;=50</t>
+  </si>
+  <si>
+    <t>.&gt;0 and .&lt;=30</t>
   </si>
 </sst>
 </file>
@@ -6401,9 +6398,9 @@
   </sheetPr>
   <dimension ref="A1:AH103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D102" sqref="D102"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <pane xSplit="4" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="M66" sqref="M66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6530,7 +6527,7 @@
         <v>1446</v>
       </c>
       <c r="C2" t="s">
-        <v>1682</v>
+        <v>1678</v>
       </c>
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.25">
@@ -6538,19 +6535,19 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>1683</v>
+        <v>1679</v>
       </c>
       <c r="C3" t="s">
-        <v>1684</v>
+        <v>1680</v>
       </c>
       <c r="F3" t="s">
-        <v>1631</v>
+        <v>1629</v>
       </c>
       <c r="G3" t="s">
         <v>116</v>
       </c>
       <c r="H3" t="s">
-        <v>1685</v>
+        <v>1681</v>
       </c>
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.25">
@@ -6567,7 +6564,7 @@
         <v>1457</v>
       </c>
       <c r="F4" t="s">
-        <v>1631</v>
+        <v>1629</v>
       </c>
       <c r="G4" t="s">
         <v>116</v>
@@ -6587,7 +6584,7 @@
         <v>1450</v>
       </c>
       <c r="F5" t="s">
-        <v>1633</v>
+        <v>1631</v>
       </c>
       <c r="G5" t="s">
         <v>116</v>
@@ -6629,10 +6626,10 @@
         <v>1448</v>
       </c>
       <c r="D8" t="s">
-        <v>1687</v>
+        <v>1683</v>
       </c>
       <c r="F8" t="s">
-        <v>1631</v>
+        <v>1629</v>
       </c>
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.25">
@@ -6640,13 +6637,13 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>1688</v>
+        <v>1684</v>
       </c>
       <c r="C9" t="s">
-        <v>1689</v>
+        <v>1685</v>
       </c>
       <c r="F9" t="s">
-        <v>1700</v>
+        <v>1696</v>
       </c>
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.25">
@@ -6660,13 +6657,13 @@
         <v>1454</v>
       </c>
       <c r="F10" t="s">
-        <v>1700</v>
+        <v>1696</v>
       </c>
       <c r="L10" t="s">
-        <v>1672</v>
+        <v>1668</v>
       </c>
       <c r="M10" t="s">
-        <v>1673</v>
+        <v>1669</v>
       </c>
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.25">
@@ -6680,10 +6677,10 @@
         <v>1456</v>
       </c>
       <c r="D11" t="s">
-        <v>1686</v>
+        <v>1682</v>
       </c>
       <c r="F11" t="s">
-        <v>1633</v>
+        <v>1631</v>
       </c>
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.25">
@@ -6727,7 +6724,7 @@
         <v>1483</v>
       </c>
       <c r="F17" t="s">
-        <v>1701</v>
+        <v>1697</v>
       </c>
       <c r="G17" t="s">
         <v>116</v>
@@ -6750,7 +6747,7 @@
         <v>1473</v>
       </c>
       <c r="F18" t="s">
-        <v>1701</v>
+        <v>1697</v>
       </c>
       <c r="G18" t="s">
         <v>116</v>
@@ -6770,7 +6767,7 @@
         <v>1469</v>
       </c>
       <c r="F19" t="s">
-        <v>1634</v>
+        <v>1632</v>
       </c>
       <c r="G19" t="s">
         <v>116</v>
@@ -6784,25 +6781,25 @@
         <v>6</v>
       </c>
       <c r="B20" t="s">
-        <v>1581</v>
+        <v>1579</v>
       </c>
       <c r="C20" t="s">
-        <v>1582</v>
+        <v>1580</v>
       </c>
       <c r="F20" t="s">
-        <v>1631</v>
+        <v>1629</v>
       </c>
       <c r="G20" t="s">
         <v>116</v>
       </c>
       <c r="H20" t="s">
-        <v>1711</v>
+        <v>1707</v>
       </c>
       <c r="L20" t="s">
         <v>1536</v>
       </c>
       <c r="M20" t="s">
-        <v>1583</v>
+        <v>1581</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
@@ -6816,7 +6813,7 @@
         <v>1477</v>
       </c>
       <c r="F21" t="s">
-        <v>1631</v>
+        <v>1629</v>
       </c>
       <c r="L21" t="s">
         <v>1536</v>
@@ -6825,7 +6822,7 @@
         <v>1535</v>
       </c>
       <c r="N21" t="s">
-        <v>1712</v>
+        <v>1708</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
@@ -6839,24 +6836,24 @@
         <v>1479</v>
       </c>
       <c r="F22" t="s">
-        <v>1633</v>
+        <v>1631</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>1692</v>
+        <v>1688</v>
       </c>
       <c r="B23" t="s">
-        <v>1690</v>
+        <v>1686</v>
       </c>
       <c r="C23" t="s">
-        <v>1690</v>
+        <v>1686</v>
       </c>
       <c r="D23" t="s">
-        <v>1704</v>
+        <v>1700</v>
       </c>
       <c r="F23" t="s">
-        <v>1693</v>
+        <v>1689</v>
       </c>
       <c r="J23" t="b">
         <v>0</v>
@@ -6864,19 +6861,19 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>1692</v>
+        <v>1688</v>
       </c>
       <c r="B24" t="s">
-        <v>1691</v>
+        <v>1687</v>
       </c>
       <c r="C24" t="s">
-        <v>1691</v>
+        <v>1687</v>
       </c>
       <c r="D24" t="s">
-        <v>1705</v>
+        <v>1701</v>
       </c>
       <c r="F24" t="s">
-        <v>1693</v>
+        <v>1689</v>
       </c>
       <c r="J24" t="b">
         <v>0</v>
@@ -6909,7 +6906,7 @@
         <v>1506</v>
       </c>
       <c r="F28" t="s">
-        <v>1634</v>
+        <v>1632</v>
       </c>
       <c r="J28">
         <v>0</v>
@@ -6926,7 +6923,7 @@
         <v>1507</v>
       </c>
       <c r="F29" t="s">
-        <v>1634</v>
+        <v>1632</v>
       </c>
       <c r="J29">
         <v>0</v>
@@ -6943,7 +6940,7 @@
         <v>1508</v>
       </c>
       <c r="F30" t="s">
-        <v>1634</v>
+        <v>1632</v>
       </c>
       <c r="J30">
         <v>0</v>
@@ -6960,7 +6957,7 @@
         <v>1509</v>
       </c>
       <c r="F31" t="s">
-        <v>1634</v>
+        <v>1632</v>
       </c>
       <c r="J31">
         <v>0</v>
@@ -6977,7 +6974,7 @@
         <v>1510</v>
       </c>
       <c r="F32" t="s">
-        <v>1634</v>
+        <v>1632</v>
       </c>
       <c r="J32">
         <v>0</v>
@@ -7000,7 +6997,7 @@
         <v>116</v>
       </c>
       <c r="K33" t="s">
-        <v>1695</v>
+        <v>1691</v>
       </c>
       <c r="L33" t="s">
         <v>1518</v>
@@ -7036,7 +7033,7 @@
         <v>1514</v>
       </c>
       <c r="F37" t="s">
-        <v>1634</v>
+        <v>1632</v>
       </c>
       <c r="J37">
         <v>0</v>
@@ -7053,7 +7050,7 @@
         <v>1515</v>
       </c>
       <c r="F38" t="s">
-        <v>1634</v>
+        <v>1632</v>
       </c>
       <c r="J38">
         <v>0</v>
@@ -7070,7 +7067,7 @@
         <v>1516</v>
       </c>
       <c r="F39" t="s">
-        <v>1634</v>
+        <v>1632</v>
       </c>
       <c r="J39">
         <v>0</v>
@@ -7087,7 +7084,7 @@
         <v>1517</v>
       </c>
       <c r="F40" t="s">
-        <v>1634</v>
+        <v>1632</v>
       </c>
       <c r="J40">
         <v>0</v>
@@ -7110,7 +7107,7 @@
         <v>116</v>
       </c>
       <c r="K41" t="s">
-        <v>1696</v>
+        <v>1692</v>
       </c>
       <c r="L41" t="s">
         <v>1505</v>
@@ -7143,13 +7140,13 @@
         <v>27</v>
       </c>
       <c r="B45" t="s">
-        <v>1699</v>
+        <v>1695</v>
       </c>
       <c r="C45" t="s">
-        <v>1637</v>
+        <v>1635</v>
       </c>
       <c r="F45" t="s">
-        <v>1632</v>
+        <v>1630</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
@@ -7163,7 +7160,7 @@
         <v>1527</v>
       </c>
       <c r="F46" t="s">
-        <v>1700</v>
+        <v>1696</v>
       </c>
       <c r="L46" t="s">
         <v>1537</v>
@@ -7183,13 +7180,13 @@
         <v>1529</v>
       </c>
       <c r="F47" t="s">
-        <v>1631</v>
+        <v>1629</v>
       </c>
       <c r="G47" t="s">
-        <v>1674</v>
+        <v>1670</v>
       </c>
       <c r="H47" t="s">
-        <v>1675</v>
+        <v>1671</v>
       </c>
       <c r="L47" t="s">
         <v>1539</v>
@@ -7209,16 +7206,16 @@
         <v>1533</v>
       </c>
       <c r="D48" t="s">
-        <v>1679</v>
+        <v>1675</v>
       </c>
       <c r="F48" t="s">
-        <v>1635</v>
+        <v>1633</v>
       </c>
       <c r="G48" t="s">
-        <v>1674</v>
+        <v>1670</v>
       </c>
       <c r="H48" t="s">
-        <v>1675</v>
+        <v>1671</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
@@ -7232,16 +7229,16 @@
         <v>1543</v>
       </c>
       <c r="D49" t="s">
-        <v>1680</v>
+        <v>1676</v>
       </c>
       <c r="F49" t="s">
-        <v>1635</v>
+        <v>1633</v>
       </c>
       <c r="G49" t="s">
-        <v>1674</v>
+        <v>1670</v>
       </c>
       <c r="H49" t="s">
-        <v>1675</v>
+        <v>1671</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
@@ -7255,16 +7252,16 @@
         <v>1534</v>
       </c>
       <c r="D50" t="s">
-        <v>1681</v>
+        <v>1677</v>
       </c>
       <c r="F50" t="s">
-        <v>1635</v>
+        <v>1633</v>
       </c>
       <c r="G50" t="s">
-        <v>1674</v>
+        <v>1670</v>
       </c>
       <c r="H50" t="s">
-        <v>1675</v>
+        <v>1671</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
@@ -7296,13 +7293,13 @@
         <v>27</v>
       </c>
       <c r="B55" t="s">
-        <v>1698</v>
+        <v>1694</v>
       </c>
       <c r="C55" t="s">
-        <v>1638</v>
+        <v>1636</v>
       </c>
       <c r="F55" t="s">
-        <v>1631</v>
+        <v>1629</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
@@ -7333,10 +7330,10 @@
         <v>1548</v>
       </c>
       <c r="G57" t="s">
-        <v>1676</v>
+        <v>1672</v>
       </c>
       <c r="H57" t="s">
-        <v>1675</v>
+        <v>1671</v>
       </c>
       <c r="L57" t="s">
         <v>1556</v>
@@ -7356,10 +7353,10 @@
         <v>1549</v>
       </c>
       <c r="G58" t="s">
-        <v>1676</v>
+        <v>1672</v>
       </c>
       <c r="H58" t="s">
-        <v>1675</v>
+        <v>1671</v>
       </c>
       <c r="L58" t="s">
         <v>1557</v>
@@ -7379,10 +7376,10 @@
         <v>1550</v>
       </c>
       <c r="G59" t="s">
-        <v>1676</v>
+        <v>1672</v>
       </c>
       <c r="H59" t="s">
-        <v>1675</v>
+        <v>1671</v>
       </c>
       <c r="L59" t="s">
         <v>1558</v>
@@ -7420,13 +7417,13 @@
         <v>27</v>
       </c>
       <c r="B64" t="s">
-        <v>1697</v>
+        <v>1693</v>
       </c>
       <c r="C64" t="s">
-        <v>1639</v>
+        <v>1637</v>
       </c>
       <c r="F64" t="s">
-        <v>1633</v>
+        <v>1631</v>
       </c>
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.25">
@@ -7440,13 +7437,13 @@
         <v>1568</v>
       </c>
       <c r="F65" t="s">
-        <v>1640</v>
+        <v>1638</v>
       </c>
       <c r="G65" t="s">
-        <v>1677</v>
+        <v>1673</v>
       </c>
       <c r="H65" t="s">
-        <v>1675</v>
+        <v>1671</v>
       </c>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.25">
@@ -7460,10 +7457,10 @@
         <v>1527</v>
       </c>
       <c r="L66" t="s">
-        <v>1578</v>
+        <v>1712</v>
       </c>
       <c r="M66" t="s">
-        <v>1577</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.25">
@@ -7477,13 +7474,13 @@
         <v>1573</v>
       </c>
       <c r="G67" t="s">
-        <v>1677</v>
+        <v>1673</v>
       </c>
       <c r="H67" t="s">
-        <v>1675</v>
+        <v>1671</v>
       </c>
       <c r="L67" t="s">
-        <v>1579</v>
+        <v>1577</v>
       </c>
       <c r="M67" t="s">
         <v>1576</v>
@@ -7500,13 +7497,13 @@
         <v>1574</v>
       </c>
       <c r="G68" t="s">
-        <v>1677</v>
+        <v>1673</v>
       </c>
       <c r="H68" t="s">
-        <v>1675</v>
+        <v>1671</v>
       </c>
       <c r="L68" t="s">
-        <v>1579</v>
+        <v>1577</v>
       </c>
       <c r="M68" t="s">
         <v>1576</v>
@@ -7523,13 +7520,13 @@
         <v>1575</v>
       </c>
       <c r="G69" t="s">
-        <v>1677</v>
+        <v>1673</v>
       </c>
       <c r="H69" t="s">
-        <v>1675</v>
+        <v>1671</v>
       </c>
       <c r="L69" t="s">
-        <v>1579</v>
+        <v>1577</v>
       </c>
       <c r="M69" t="s">
         <v>1576</v>
@@ -7550,176 +7547,176 @@
         <v>27</v>
       </c>
       <c r="B73" t="s">
-        <v>1584</v>
+        <v>1582</v>
       </c>
       <c r="C73" t="s">
-        <v>1585</v>
+        <v>1583</v>
       </c>
       <c r="F73" t="s">
-        <v>1641</v>
+        <v>1639</v>
       </c>
       <c r="N73" t="s">
-        <v>1666</v>
+        <v>1664</v>
       </c>
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>1586</v>
+        <v>1584</v>
       </c>
       <c r="B74" t="s">
-        <v>1587</v>
+        <v>1585</v>
       </c>
       <c r="C74" t="s">
-        <v>1598</v>
+        <v>1596</v>
       </c>
       <c r="D74" t="s">
-        <v>1702</v>
+        <v>1698</v>
       </c>
       <c r="F74" t="s">
-        <v>1642</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
+        <v>1584</v>
+      </c>
+      <c r="B75" t="s">
         <v>1586</v>
       </c>
-      <c r="B75" t="s">
-        <v>1588</v>
-      </c>
       <c r="C75" t="s">
-        <v>1599</v>
+        <v>1597</v>
       </c>
       <c r="D75" t="s">
-        <v>1703</v>
+        <v>1699</v>
       </c>
       <c r="F75" t="s">
-        <v>1642</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>1586</v>
+        <v>1584</v>
       </c>
       <c r="B76" t="s">
-        <v>1589</v>
+        <v>1587</v>
       </c>
       <c r="C76" t="s">
-        <v>1600</v>
+        <v>1598</v>
       </c>
       <c r="F76" t="s">
-        <v>1642</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>1586</v>
+        <v>1584</v>
       </c>
       <c r="B77" t="s">
-        <v>1590</v>
+        <v>1588</v>
       </c>
       <c r="C77" t="s">
-        <v>1601</v>
+        <v>1599</v>
       </c>
       <c r="F77" t="s">
-        <v>1642</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>1586</v>
+        <v>1584</v>
       </c>
       <c r="B78" t="s">
-        <v>1591</v>
+        <v>1589</v>
       </c>
       <c r="C78" t="s">
-        <v>1602</v>
+        <v>1600</v>
       </c>
       <c r="F78" t="s">
-        <v>1642</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>1586</v>
+        <v>1584</v>
       </c>
       <c r="B79" t="s">
-        <v>1592</v>
+        <v>1590</v>
       </c>
       <c r="C79" t="s">
-        <v>1603</v>
+        <v>1601</v>
       </c>
       <c r="F79" t="s">
-        <v>1642</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>1586</v>
+        <v>1584</v>
       </c>
       <c r="B80" t="s">
-        <v>1593</v>
+        <v>1591</v>
       </c>
       <c r="C80" t="s">
-        <v>1604</v>
+        <v>1602</v>
       </c>
       <c r="F80" t="s">
-        <v>1642</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>1586</v>
+        <v>1584</v>
       </c>
       <c r="B81" t="s">
-        <v>1594</v>
+        <v>1592</v>
       </c>
       <c r="C81" t="s">
-        <v>1605</v>
+        <v>1603</v>
       </c>
       <c r="F81" t="s">
-        <v>1642</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>1586</v>
+        <v>1584</v>
       </c>
       <c r="B82" t="s">
-        <v>1595</v>
+        <v>1593</v>
       </c>
       <c r="C82" t="s">
-        <v>1606</v>
+        <v>1604</v>
       </c>
       <c r="F82" t="s">
-        <v>1642</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>1586</v>
+        <v>1584</v>
       </c>
       <c r="B83" t="s">
-        <v>1596</v>
+        <v>1594</v>
       </c>
       <c r="C83" t="s">
-        <v>1607</v>
+        <v>1605</v>
       </c>
       <c r="F83" t="s">
-        <v>1642</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>1586</v>
+        <v>1584</v>
       </c>
       <c r="B84" t="s">
-        <v>1597</v>
+        <v>1595</v>
       </c>
       <c r="C84" t="s">
-        <v>1608</v>
+        <v>1606</v>
       </c>
       <c r="F84" t="s">
-        <v>1642</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.25">
@@ -7732,16 +7729,16 @@
         <v>27</v>
       </c>
       <c r="B87" t="s">
-        <v>1645</v>
+        <v>1643</v>
       </c>
       <c r="C87" t="s">
-        <v>1646</v>
+        <v>1644</v>
       </c>
       <c r="F87" t="s">
-        <v>1636</v>
+        <v>1634</v>
       </c>
       <c r="N87" t="s">
-        <v>1665</v>
+        <v>1663</v>
       </c>
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.25">
@@ -7749,25 +7746,25 @@
         <v>6</v>
       </c>
       <c r="B88" t="s">
-        <v>1647</v>
+        <v>1645</v>
       </c>
       <c r="C88" t="s">
-        <v>1652</v>
+        <v>1650</v>
       </c>
       <c r="F88" t="s">
-        <v>1700</v>
+        <v>1696</v>
       </c>
       <c r="G88" t="s">
-        <v>1665</v>
+        <v>1663</v>
       </c>
       <c r="H88" t="s">
-        <v>1678</v>
+        <v>1674</v>
       </c>
       <c r="L88" t="s">
-        <v>1657</v>
+        <v>1655</v>
       </c>
       <c r="M88" t="s">
-        <v>1710</v>
+        <v>1706</v>
       </c>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.25">
@@ -7775,25 +7772,25 @@
         <v>6</v>
       </c>
       <c r="B89" t="s">
-        <v>1648</v>
+        <v>1646</v>
       </c>
       <c r="C89" t="s">
-        <v>1653</v>
+        <v>1651</v>
       </c>
       <c r="F89" t="s">
-        <v>1700</v>
+        <v>1696</v>
       </c>
       <c r="G89" t="s">
-        <v>1665</v>
+        <v>1663</v>
       </c>
       <c r="H89" t="s">
-        <v>1678</v>
+        <v>1674</v>
       </c>
       <c r="L89" t="s">
-        <v>1657</v>
+        <v>1655</v>
       </c>
       <c r="M89" t="s">
-        <v>1710</v>
+        <v>1706</v>
       </c>
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.25">
@@ -7801,25 +7798,25 @@
         <v>6</v>
       </c>
       <c r="B90" t="s">
-        <v>1649</v>
+        <v>1647</v>
       </c>
       <c r="C90" t="s">
-        <v>1654</v>
+        <v>1652</v>
       </c>
       <c r="F90" t="s">
-        <v>1700</v>
+        <v>1696</v>
       </c>
       <c r="G90" t="s">
-        <v>1665</v>
+        <v>1663</v>
       </c>
       <c r="H90" t="s">
-        <v>1678</v>
+        <v>1674</v>
       </c>
       <c r="L90" t="s">
-        <v>1657</v>
+        <v>1655</v>
       </c>
       <c r="M90" t="s">
-        <v>1710</v>
+        <v>1706</v>
       </c>
     </row>
     <row r="91" spans="1:14" x14ac:dyDescent="0.25">
@@ -7827,19 +7824,19 @@
         <v>6</v>
       </c>
       <c r="B91" t="s">
-        <v>1650</v>
+        <v>1648</v>
       </c>
       <c r="C91" t="s">
+        <v>1653</v>
+      </c>
+      <c r="F91" t="s">
+        <v>1696</v>
+      </c>
+      <c r="L91" t="s">
         <v>1655</v>
       </c>
-      <c r="F91" t="s">
-        <v>1700</v>
-      </c>
-      <c r="L91" t="s">
-        <v>1657</v>
-      </c>
       <c r="M91" t="s">
-        <v>1710</v>
+        <v>1706</v>
       </c>
     </row>
     <row r="92" spans="1:14" x14ac:dyDescent="0.25">
@@ -7847,19 +7844,19 @@
         <v>6</v>
       </c>
       <c r="B92" t="s">
-        <v>1651</v>
+        <v>1649</v>
       </c>
       <c r="C92" t="s">
-        <v>1656</v>
+        <v>1654</v>
       </c>
       <c r="F92" t="s">
-        <v>1700</v>
+        <v>1696</v>
       </c>
       <c r="L92" t="s">
-        <v>1657</v>
+        <v>1655</v>
       </c>
       <c r="M92" t="s">
-        <v>1710</v>
+        <v>1706</v>
       </c>
     </row>
     <row r="93" spans="1:14" x14ac:dyDescent="0.25">
@@ -7872,10 +7869,10 @@
         <v>31</v>
       </c>
       <c r="B95" t="s">
-        <v>1658</v>
+        <v>1656</v>
       </c>
       <c r="C95" t="s">
-        <v>1658</v>
+        <v>1656</v>
       </c>
       <c r="F95" t="s">
         <v>82</v>
@@ -7886,13 +7883,13 @@
         <v>27</v>
       </c>
       <c r="B96" t="s">
-        <v>1659</v>
+        <v>1657</v>
       </c>
       <c r="C96" t="s">
-        <v>1660</v>
+        <v>1658</v>
       </c>
       <c r="F96" t="s">
-        <v>1632</v>
+        <v>1630</v>
       </c>
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.25">
@@ -7900,22 +7897,22 @@
         <v>6</v>
       </c>
       <c r="B97" t="s">
-        <v>1706</v>
+        <v>1702</v>
       </c>
       <c r="C97" t="s">
-        <v>1707</v>
+        <v>1703</v>
       </c>
       <c r="D97" t="s">
-        <v>1709</v>
+        <v>1705</v>
       </c>
       <c r="F97" t="s">
-        <v>1700</v>
+        <v>1696</v>
       </c>
       <c r="L97" t="s">
-        <v>1670</v>
+        <v>1711</v>
       </c>
       <c r="M97" t="s">
-        <v>1667</v>
+        <v>1710</v>
       </c>
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.25">
@@ -7923,28 +7920,28 @@
         <v>6</v>
       </c>
       <c r="B98" t="s">
+        <v>1659</v>
+      </c>
+      <c r="C98" t="s">
         <v>1661</v>
       </c>
-      <c r="C98" t="s">
-        <v>1663</v>
-      </c>
       <c r="D98" t="s">
-        <v>1708</v>
+        <v>1704</v>
       </c>
       <c r="F98" t="s">
-        <v>1700</v>
+        <v>1696</v>
       </c>
       <c r="G98" t="s">
-        <v>1713</v>
+        <v>1709</v>
       </c>
       <c r="H98" t="s">
-        <v>1675</v>
+        <v>1671</v>
       </c>
       <c r="L98" t="s">
-        <v>1579</v>
+        <v>1539</v>
       </c>
       <c r="M98" t="s">
-        <v>1668</v>
+        <v>1665</v>
       </c>
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.25">
@@ -7952,28 +7949,28 @@
         <v>6</v>
       </c>
       <c r="B99" t="s">
+        <v>1660</v>
+      </c>
+      <c r="C99" t="s">
         <v>1662</v>
       </c>
-      <c r="C99" t="s">
-        <v>1664</v>
-      </c>
       <c r="D99" t="s">
-        <v>1708</v>
+        <v>1704</v>
       </c>
       <c r="F99" t="s">
-        <v>1700</v>
+        <v>1696</v>
       </c>
       <c r="G99" t="s">
-        <v>1713</v>
+        <v>1709</v>
       </c>
       <c r="H99" t="s">
-        <v>1675</v>
+        <v>1671</v>
       </c>
       <c r="L99" t="s">
-        <v>1671</v>
+        <v>1667</v>
       </c>
       <c r="M99" t="s">
-        <v>1669</v>
+        <v>1666</v>
       </c>
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.25">
@@ -8130,7 +8127,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>1694</v>
+        <v>1690</v>
       </c>
       <c r="B9" t="b">
         <v>0</v>
@@ -8141,7 +8138,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>1694</v>
+        <v>1690</v>
       </c>
       <c r="B10" t="b">
         <v>1</v>
@@ -8323,238 +8320,238 @@
         <v>1565</v>
       </c>
       <c r="C29" t="s">
-        <v>1580</v>
+        <v>1578</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>1609</v>
+        <v>1607</v>
       </c>
       <c r="B31">
         <v>0.03</v>
       </c>
       <c r="C31" s="41" t="s">
-        <v>1611</v>
+        <v>1609</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>1609</v>
+        <v>1607</v>
       </c>
       <c r="B32">
         <v>1.03</v>
       </c>
       <c r="C32" s="41" t="s">
-        <v>1612</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>1609</v>
+        <v>1607</v>
       </c>
       <c r="B33">
         <v>3</v>
       </c>
       <c r="C33" s="41" t="s">
-        <v>1613</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>1609</v>
+        <v>1607</v>
       </c>
       <c r="B34">
         <v>4.8499999999999996</v>
       </c>
       <c r="C34" s="41" t="s">
-        <v>1614</v>
+        <v>1612</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>1609</v>
+        <v>1607</v>
       </c>
       <c r="B35">
         <v>6.85</v>
       </c>
       <c r="C35" s="41" t="s">
-        <v>1615</v>
+        <v>1613</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>1609</v>
+        <v>1607</v>
       </c>
       <c r="B36">
         <v>9.65</v>
       </c>
       <c r="C36" s="41" t="s">
-        <v>1616</v>
+        <v>1614</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>1609</v>
+        <v>1607</v>
       </c>
       <c r="B37">
         <v>13.65</v>
       </c>
       <c r="C37" s="41" t="s">
-        <v>1617</v>
+        <v>1615</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>1609</v>
+        <v>1607</v>
       </c>
       <c r="B38">
         <v>19.3</v>
       </c>
       <c r="C38" s="41" t="s">
-        <v>1618</v>
+        <v>1616</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>1609</v>
+        <v>1607</v>
       </c>
       <c r="B39">
         <v>27.3</v>
       </c>
       <c r="C39" s="41" t="s">
-        <v>1619</v>
+        <v>1617</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>1609</v>
+        <v>1607</v>
       </c>
       <c r="B40">
         <v>38.5</v>
       </c>
       <c r="C40" s="41" t="s">
-        <v>1620</v>
+        <v>1618</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>1609</v>
+        <v>1607</v>
       </c>
       <c r="B41">
         <v>54.5</v>
       </c>
       <c r="C41" s="41" t="s">
-        <v>1621</v>
+        <v>1619</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>1609</v>
+        <v>1607</v>
       </c>
       <c r="B42">
         <v>77</v>
       </c>
       <c r="C42" s="41" t="s">
-        <v>1622</v>
+        <v>1620</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>1609</v>
+        <v>1607</v>
       </c>
       <c r="B43">
         <v>109</v>
       </c>
       <c r="C43" s="41" t="s">
-        <v>1623</v>
+        <v>1621</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>1609</v>
+        <v>1607</v>
       </c>
       <c r="B44">
         <v>154</v>
       </c>
       <c r="C44" s="41" t="s">
-        <v>1624</v>
+        <v>1622</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>1609</v>
+        <v>1607</v>
       </c>
       <c r="B45">
         <v>218</v>
       </c>
       <c r="C45" s="41" t="s">
-        <v>1625</v>
+        <v>1623</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>1609</v>
+        <v>1607</v>
       </c>
       <c r="B46">
         <v>309</v>
       </c>
       <c r="C46" s="41" t="s">
-        <v>1626</v>
+        <v>1624</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>1609</v>
+        <v>1607</v>
       </c>
       <c r="B47">
         <v>437</v>
       </c>
       <c r="C47" s="41" t="s">
-        <v>1627</v>
+        <v>1625</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>1609</v>
+        <v>1607</v>
       </c>
       <c r="B48">
         <v>618</v>
       </c>
       <c r="C48" s="41" t="s">
-        <v>1628</v>
+        <v>1626</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>1609</v>
+        <v>1607</v>
       </c>
       <c r="B49">
         <v>874</v>
       </c>
       <c r="C49" s="41" t="s">
-        <v>1629</v>
+        <v>1627</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>1609</v>
+        <v>1607</v>
       </c>
       <c r="B50">
         <v>1024</v>
       </c>
       <c r="C50" s="41" t="s">
-        <v>1644</v>
+        <v>1642</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>1609</v>
+        <v>1607</v>
       </c>
       <c r="B51" t="s">
-        <v>1610</v>
+        <v>1608</v>
       </c>
       <c r="C51" s="41" t="s">
-        <v>1643</v>
+        <v>1641</v>
       </c>
     </row>
   </sheetData>
@@ -8614,7 +8611,7 @@
         <v>1522</v>
       </c>
       <c r="G2" t="s">
-        <v>1630</v>
+        <v>1628</v>
       </c>
       <c r="H2" t="s">
         <v>116</v>

</xml_diff>